<commit_message>
improved version wit main loop and output fix
</commit_message>
<xml_diff>
--- a/dell/summary_report.xlsx
+++ b/dell/summary_report.xlsx
@@ -14,45 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Service Tag</t>
   </si>
   <si>
-    <t>C1MM2S2</t>
+    <t>C1VV2S2</t>
   </si>
   <si>
     <t>IP addres</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
+    <t>0.0.0.0</t>
   </si>
   <si>
     <t>Conf passed</t>
   </si>
   <si>
-    <t>1593</t>
+    <t>1602</t>
   </si>
   <si>
     <t>Conf error</t>
   </si>
   <si>
-    <t>4</t>
+    <t>0</t>
   </si>
   <si>
     <t>HW passed</t>
   </si>
   <si>
-    <t>13</t>
+    <t>70</t>
   </si>
   <si>
     <t>HW error</t>
   </si>
   <si>
-    <t>58</t>
+    <t>1</t>
   </si>
   <si>
     <t>C1WN2S2</t>
+  </si>
+  <si>
+    <t>1601</t>
+  </si>
+  <si>
+    <t>71</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -480,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -488,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -496,7 +502,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>